<commit_message>
Update - Mise à jour du traitement du fichier de produits
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\sheaft\app\Sheaft.Resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noelm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89E0BA6-BB1F-476E-84AF-B6AA2B3363CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07AB8E-CB37-4843-B72E-3FBA5A6576C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Référence</t>
   </si>
@@ -47,23 +47,42 @@
     <t>Prix HT</t>
   </si>
   <si>
-    <t>TVA (en %)</t>
-  </si>
-  <si>
-    <t>Poids (en gramme, optionel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catégories (choisir parmi: Fruits et légumes,Viandes,Laitages,Alcool,Bio. Attention à bien séparer les catégories par une virgule) </t>
-  </si>
-  <si>
-    <t>Disponible à la vente (Oui, Non)</t>
+    <t>Conditionnement
+(Poids, Botte, Boite, Bouquet, Pièce)</t>
+  </si>
+  <si>
+    <t>TVA % 
+(5.5, 10 ou 20)</t>
+  </si>
+  <si>
+    <t>Catégorie
+(Fruits et légumes,Viandes,Poissons,Laitages,Boisson,Epicerie)</t>
+  </si>
+  <si>
+    <t>Agriculture Bio
+(Oui, Non)</t>
+  </si>
+  <si>
+    <t>Unité de mesure (ml, L, g, kg) 
+Uniquement si conditionnement = Poids</t>
+  </si>
+  <si>
+    <t>Quantité ou poids du conditionnement (exemple: 5)</t>
+  </si>
+  <si>
+    <t>Disponible à la vente 
+(Oui, Non)</t>
+  </si>
+  <si>
+    <t>Poids total 
+(en gramme, optionel)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,16 +90,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,13 +121,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -119,17 +166,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H2" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D92E2E28-3FCD-4E60-9218-DD51D90B6F26}" name="Référence"/>
     <tableColumn id="2" xr3:uid="{CB863275-704A-4D0D-ACB9-A301D1DFFF79}" name="Nom"/>
-    <tableColumn id="3" xr3:uid="{BB4AD7E6-4253-4107-A75F-DACF8F14548E}" name="Description"/>
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
-    <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA (en %)"/>
-    <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Poids (en gramme, optionel)"/>
-    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente (Oui, Non)"/>
-    <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégories (choisir parmi: Fruits et légumes,Viandes,Laitages,Alcool,Bio. Attention à bien séparer les catégories par une virgule) "/>
+    <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % _x000a_(5.5, 10 ou 20)"/>
+    <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement_x000a_(Poids, Botte, Boite, Bouquet, Pièce)"/>
+    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Quantité ou poids du conditionnement (exemple: 5)"/>
+    <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure (ml, L, g, kg) _x000a_Uniquement si conditionnement = Poids"/>
+    <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie_x000a_(Fruits et légumes,Viandes,Poissons,Laitages,Boisson,Epicerie)"/>
+    <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio_x000a_(Oui, Non)"/>
+    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente _x000a_(Oui, Non)"/>
+    <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Description"/>
+    <tableColumn id="12" xr3:uid="{232EFC38-45BD-417B-956E-A3C32917C5D6}" name="Poids total _x000a_(en gramme, optionel)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -432,24 +483,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="67.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,24 +514,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update - Mise à jour du fichier excel
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -5,35 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noelm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07AB8E-CB37-4843-B72E-3FBA5A6576C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F5DB9-26E0-4BA1-87EF-6BCEAC975236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
+    <sheet name="Listes" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="liste_bool">Tableau6[Boolean]</definedName>
+    <definedName name="liste_categorie">Tableau5[Catégorie]</definedName>
+    <definedName name="liste_conditionnement">Tableau2[Conditionnement]</definedName>
+    <definedName name="liste_tva">Tableau1[TVA]</definedName>
+    <definedName name="liste_um">Tableau3[Unité de mesure]</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Référence</t>
   </si>
@@ -47,35 +47,86 @@
     <t>Prix HT</t>
   </si>
   <si>
-    <t>Conditionnement
-(Poids, Botte, Boite, Bouquet, Pièce)</t>
-  </si>
-  <si>
-    <t>TVA % 
-(5.5, 10 ou 20)</t>
-  </si>
-  <si>
-    <t>Catégorie
-(Fruits et légumes,Viandes,Poissons,Laitages,Boisson,Epicerie)</t>
-  </si>
-  <si>
-    <t>Agriculture Bio
-(Oui, Non)</t>
-  </si>
-  <si>
-    <t>Unité de mesure (ml, L, g, kg) 
+    <t>Quantité ou poids du conditionnement (exemple: 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVA % </t>
+  </si>
+  <si>
+    <t>TVA</t>
+  </si>
+  <si>
+    <t>Conditionnement</t>
+  </si>
+  <si>
+    <t>Unité de mesure</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Poids</t>
+  </si>
+  <si>
+    <t>Botte</t>
+  </si>
+  <si>
+    <t>Pièce</t>
+  </si>
+  <si>
+    <t>Boîte</t>
+  </si>
+  <si>
+    <t>Bouquet</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Unité de mesure
 Uniquement si conditionnement = Poids</t>
   </si>
   <si>
-    <t>Quantité ou poids du conditionnement (exemple: 5)</t>
-  </si>
-  <si>
-    <t>Disponible à la vente 
-(Oui, Non)</t>
-  </si>
-  <si>
-    <t>Poids total 
-(en gramme, optionel)</t>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>Fruits et légumes</t>
+  </si>
+  <si>
+    <t>Boisson</t>
+  </si>
+  <si>
+    <t>Viande</t>
+  </si>
+  <si>
+    <t>Épicerie</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Agriculture Bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponible à la vente </t>
+  </si>
+  <si>
+    <t>Oeufs et produits laitiers</t>
   </si>
 </sst>
 </file>
@@ -166,23 +217,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:L1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D92E2E28-3FCD-4E60-9218-DD51D90B6F26}" name="Référence"/>
     <tableColumn id="2" xr3:uid="{CB863275-704A-4D0D-ACB9-A301D1DFFF79}" name="Nom"/>
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
-    <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % _x000a_(5.5, 10 ou 20)"/>
-    <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement_x000a_(Poids, Botte, Boite, Bouquet, Pièce)"/>
+    <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % "/>
+    <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement"/>
     <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Quantité ou poids du conditionnement (exemple: 5)"/>
-    <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure (ml, L, g, kg) _x000a_Uniquement si conditionnement = Poids"/>
-    <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie_x000a_(Fruits et légumes,Viandes,Poissons,Laitages,Boisson,Epicerie)"/>
-    <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio_x000a_(Oui, Non)"/>
-    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente _x000a_(Oui, Non)"/>
+    <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_Uniquement si conditionnement = Poids"/>
+    <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie"/>
+    <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio"/>
+    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente "/>
     <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Description"/>
-    <tableColumn id="12" xr3:uid="{232EFC38-45BD-417B-956E-A3C32917C5D6}" name="Poids total _x000a_(en gramme, optionel)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88C7E208-3AC1-451F-B7B8-493E27854359}" name="Tableau1" displayName="Tableau1" ref="A1:A4" totalsRowShown="0">
+  <autoFilter ref="A1:A4" xr:uid="{263B2DA4-B8DA-4C48-98D1-DD15658A8721}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D845EE2E-9442-4F67-AB37-3AFDB6862999}" name="TVA"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{118CB03D-25DF-42FE-B29A-A111E35E3C12}" name="Tableau2" displayName="Tableau2" ref="C1:C6" totalsRowShown="0">
+  <autoFilter ref="C1:C6" xr:uid="{784D7B01-7C02-4731-A9FA-72B7824767CF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C6">
+    <sortCondition ref="C2:C6"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{773A62E2-383A-4184-B887-9F9C1D4BDD1A}" name="Conditionnement"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F98A693-E441-414B-AC52-72C75E56F8B4}" name="Tableau3" displayName="Tableau3" ref="E1:E5" totalsRowShown="0">
+  <autoFilter ref="E1:E5" xr:uid="{2451232D-0318-41AD-9BCC-A8D23DB3E0DE}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2153DFFB-89FB-413C-9739-97719328EE13}" name="Unité de mesure"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{482A5A29-7639-4322-B562-2426D46250A7}" name="Tableau5" displayName="Tableau5" ref="G1:G7" totalsRowShown="0">
+  <autoFilter ref="G1:G7" xr:uid="{C4CC0989-BC2B-4B26-8D92-EBAD3EF0C78D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G7">
+    <sortCondition ref="G2:G7"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{567C0C37-678B-423F-9212-65CEE0DFA9B1}" name="Catégorie"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{06952DEA-3EDA-4BBA-9897-A02433C64B45}" name="Tableau6" displayName="Tableau6" ref="I1:I3" totalsRowShown="0">
+  <autoFilter ref="I1:I3" xr:uid="{53C7C36B-5694-467D-986B-1E2B045AA21B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{84F91542-41F0-4837-965A-508F5ACB4D69}" name="Boolean"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -483,30 +589,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="45" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,35 +625,175 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="D2:D1048576" xr:uid="{158F52B8-4521-4DFE-85C4-7E1DDB94B372}">
+      <formula1>liste_tva</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="E2:E1048576" xr:uid="{005D2DCD-0D66-41E5-8C96-59993C5B54D5}">
+      <formula1>liste_conditionnement</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="G2:G1048576" xr:uid="{90639BCB-1565-4D42-A16B-F93A99BF7FB1}">
+      <formula1>liste_um</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="H2:H1048576" xr:uid="{363A8532-58B7-47B2-9B73-90212EFBEAE8}">
+      <formula1>liste_categorie</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="J2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
+      <formula1>liste_bool</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:I1048576" xr:uid="{8E1218FC-9D0C-4837-82CE-9B67227D53AB}">
+      <formula1>liste_bool</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="C2:C1048576" xr:uid="{0EA629EE-16BC-4DE0-87D1-6ED26E9694CF}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372973B1-2516-4285-BAE1-16E251103327}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix - Update du fichier import
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F5DB9-26E0-4BA1-87EF-6BCEAC975236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F8AFB42-EAE8-4F8C-98A0-6F520D1AC4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
@@ -99,18 +99,9 @@
 Uniquement si conditionnement = Poids</t>
   </si>
   <si>
-    <t>Poisson</t>
-  </si>
-  <si>
     <t>Fruits et légumes</t>
   </si>
   <si>
-    <t>Boisson</t>
-  </si>
-  <si>
-    <t>Viande</t>
-  </si>
-  <si>
     <t>Épicerie</t>
   </si>
   <si>
@@ -127,6 +118,15 @@
   </si>
   <si>
     <t>Oeufs et produits laitiers</t>
+  </si>
+  <si>
+    <t>Boissons</t>
+  </si>
+  <si>
+    <t>Poissons</t>
+  </si>
+  <si>
+    <t>Viandes</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +637,10 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="D2:D1048576" xr:uid="{158F52B8-4521-4DFE-85C4-7E1DDB94B372}">
       <formula1>liste_tva</formula1>
     </dataValidation>
@@ -661,16 +661,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="H2:H1048576" xr:uid="{363A8532-58B7-47B2-9B73-90212EFBEAE8}">
       <formula1>liste_categorie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="J2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
       <formula1>liste_bool</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:I1048576" xr:uid="{8E1218FC-9D0C-4837-82CE-9B67227D53AB}">
-      <formula1>liste_bool</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="C2:C1048576" xr:uid="{0EA629EE-16BC-4DE0-87D1-6ED26E9694CF}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576 C2:C1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -686,7 +680,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,10 +719,10 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -742,10 +736,10 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,7 +753,7 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -770,7 +764,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -778,12 +772,12 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix - Correction des index azure search
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F8AFB42-EAE8-4F8C-98A0-6F520D1AC4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03553B-A10C-4A60-A1B9-6209EEE1A4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>Prix HT</t>
   </si>
   <si>
-    <t>Quantité ou poids du conditionnement (exemple: 5)</t>
-  </si>
-  <si>
     <t xml:space="preserve">TVA % </t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>Viandes</t>
+  </si>
+  <si>
+    <t>Nombre de pièces ou poids du conditionnement</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
     <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % "/>
     <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement"/>
-    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Quantité ou poids du conditionnement (exemple: 5)"/>
+    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Nombre de pièces ou poids du conditionnement"/>
     <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_Uniquement si conditionnement = Poids"/>
     <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie"/>
     <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio"/>
@@ -592,7 +592,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,25 +622,25 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
@@ -693,19 +693,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -713,16 +713,16 @@
         <v>5.5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -730,16 +730,16 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,37 +747,37 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - Mise à jour du fichier d'import produits
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03553B-A10C-4A60-A1B9-6209EEE1A4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E9FE62-134D-4891-B216-ADDD62B9040D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
@@ -32,8 +32,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Fanny</author>
+  </authors>
+  <commentList>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{299EC857-1896-4A9F-8BC2-ED4A1B88F562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Si "Non", les consommateurs ne peuvent pas commander le produit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{4DF44008-85F2-4D6C-A614-F3287A4F68E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Si "Oui", le produit est visible dans les résultats de recherche des consommateurs.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Référence</t>
   </si>
@@ -92,48 +130,51 @@
     <t>kg</t>
   </si>
   <si>
+    <t>Fruits et légumes</t>
+  </si>
+  <si>
+    <t>Épicerie</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Agriculture Bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponible à la vente </t>
+  </si>
+  <si>
+    <t>Oeufs et produits laitiers</t>
+  </si>
+  <si>
+    <t>Boissons</t>
+  </si>
+  <si>
+    <t>Poissons</t>
+  </si>
+  <si>
+    <t>Viandes</t>
+  </si>
+  <si>
+    <t>Visible</t>
+  </si>
+  <si>
     <t>Unité de mesure
-Uniquement si conditionnement = Poids</t>
-  </si>
-  <si>
-    <t>Fruits et légumes</t>
-  </si>
-  <si>
-    <t>Épicerie</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Non</t>
-  </si>
-  <si>
-    <t>Agriculture Bio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disponible à la vente </t>
-  </si>
-  <si>
-    <t>Oeufs et produits laitiers</t>
-  </si>
-  <si>
-    <t>Boissons</t>
-  </si>
-  <si>
-    <t>Poissons</t>
-  </si>
-  <si>
-    <t>Viandes</t>
-  </si>
-  <si>
-    <t>Nombre de pièces ou poids du conditionnement</t>
+(uniquement si conditionnement = Poids)</t>
+  </si>
+  <si>
+    <t>Nombre de pièces/boîtes ou poids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +189,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -217,19 +272,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:K1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D92E2E28-3FCD-4E60-9218-DD51D90B6F26}" name="Référence"/>
     <tableColumn id="2" xr3:uid="{CB863275-704A-4D0D-ACB9-A301D1DFFF79}" name="Nom"/>
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
     <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % "/>
     <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement"/>
-    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Nombre de pièces ou poids du conditionnement"/>
-    <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_Uniquement si conditionnement = Poids"/>
+    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Nombre de pièces/boîtes ou poids"/>
+    <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_(uniquement si conditionnement = Poids)"/>
     <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie"/>
     <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio"/>
     <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente "/>
+    <tableColumn id="12" xr3:uid="{9F5B3A42-D323-4323-AACF-475CADF70BEE}" name="Visible"/>
     <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -588,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,16 +658,16 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="45" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="10" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="45" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,25 +684,28 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="D2:D1048576" xr:uid="{158F52B8-4521-4DFE-85C4-7E1DDB94B372}">
@@ -661,7 +720,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="H2:H1048576" xr:uid="{363A8532-58B7-47B2-9B73-90212EFBEAE8}">
       <formula1>liste_categorie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:K1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
       <formula1>liste_bool</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576 C2:C1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">
@@ -669,8 +728,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -719,10 +780,10 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -736,10 +797,10 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -753,7 +814,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -764,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -772,12 +833,12 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix - Modification du handling du fichier excel d'import
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E9FE62-134D-4891-B216-ADDD62B9040D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18104C5C-977B-4298-A8B6-8C6DA34E2276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
@@ -32,46 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Fanny</author>
-  </authors>
-  <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{299EC857-1896-4A9F-8BC2-ED4A1B88F562}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Si "Non", les consommateurs ne peuvent pas commander le produit.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{4DF44008-85F2-4D6C-A614-F3287A4F68E1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Si "Oui", le produit est visible dans les résultats de recherche des consommateurs.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Référence</t>
   </si>
@@ -145,9 +107,6 @@
     <t>Agriculture Bio</t>
   </si>
   <si>
-    <t xml:space="preserve">Disponible à la vente </t>
-  </si>
-  <si>
     <t>Oeufs et produits laitiers</t>
   </si>
   <si>
@@ -158,23 +117,25 @@
   </si>
   <si>
     <t>Viandes</t>
-  </si>
-  <si>
-    <t>Visible</t>
   </si>
   <si>
     <t>Unité de mesure
 (uniquement si conditionnement = Poids)</t>
   </si>
   <si>
-    <t>Nombre de pièces/boîtes ou poids</t>
+    <t>Disponible à la vente
+(si "Non", les consommateurs ne peuvent pas commander le produit)</t>
+  </si>
+  <si>
+    <t>Nombre de pièces ou poids
+(si boîte, quantité contenue)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,20 +150,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -272,20 +219,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:L1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D92E2E28-3FCD-4E60-9218-DD51D90B6F26}" name="Référence"/>
     <tableColumn id="2" xr3:uid="{CB863275-704A-4D0D-ACB9-A301D1DFFF79}" name="Nom"/>
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
     <tableColumn id="5" xr3:uid="{8A70BB56-C020-4207-B07C-3DE03E0CB4CC}" name="TVA % "/>
     <tableColumn id="3" xr3:uid="{5BAAB90B-F3FB-4A87-ACD3-4EAF5D1ADBCD}" name="Conditionnement"/>
-    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Nombre de pièces/boîtes ou poids"/>
+    <tableColumn id="10" xr3:uid="{56863EE2-1B9A-4266-B921-7391C9999176}" name="Nombre de pièces ou poids_x000a_(si boîte, quantité contenue)"/>
     <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_(uniquement si conditionnement = Poids)"/>
     <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie"/>
     <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio"/>
-    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente "/>
-    <tableColumn id="12" xr3:uid="{9F5B3A42-D323-4323-AACF-475CADF70BEE}" name="Visible"/>
+    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente_x000a_(si &quot;Non&quot;, les consommateurs ne peuvent pas commander le produit)"/>
     <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -644,11 +590,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,12 +608,12 @@
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="45" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="45" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,10 +630,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -696,16 +642,13 @@
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="D2:D1048576" xr:uid="{158F52B8-4521-4DFE-85C4-7E1DDB94B372}">
@@ -720,7 +663,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="H2:H1048576" xr:uid="{363A8532-58B7-47B2-9B73-90212EFBEAE8}">
       <formula1>liste_categorie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:K1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
       <formula1>liste_bool</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576 C2:C1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">
@@ -729,9 +672,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -780,7 +722,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -825,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,12 +775,12 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - Suppression de la colone Available du fichier d'import
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\sheaft\api\Sheaft.Resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18104C5C-977B-4298-A8B6-8C6DA34E2276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB5E5D7-853A-494A-9CA5-831B88C5893A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Référence</t>
   </si>
@@ -121,10 +121,6 @@
   <si>
     <t>Unité de mesure
 (uniquement si conditionnement = Poids)</t>
-  </si>
-  <si>
-    <t>Disponible à la vente
-(si "Non", les consommateurs ne peuvent pas commander le produit)</t>
   </si>
   <si>
     <t>Nombre de pièces ou poids
@@ -219,9 +215,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:K1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97C38175-D857-4CC4-A360-E533857C1D42}" name="Tableau4" displayName="Tableau4" ref="A1:J1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J1048576" xr:uid="{AF18564E-D743-4F97-9318-01CAB3320B59}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{D92E2E28-3FCD-4E60-9218-DD51D90B6F26}" name="Référence"/>
     <tableColumn id="2" xr3:uid="{CB863275-704A-4D0D-ACB9-A301D1DFFF79}" name="Nom"/>
     <tableColumn id="4" xr3:uid="{E6104492-A2A0-4EBB-B775-92B2C3EB0DCC}" name="Prix HT"/>
@@ -231,7 +227,6 @@
     <tableColumn id="11" xr3:uid="{F86E0392-79F8-4D1D-8AF1-1E155615B161}" name="Unité de mesure_x000a_(uniquement si conditionnement = Poids)"/>
     <tableColumn id="7" xr3:uid="{A0D230C0-C2F3-47D4-B8AC-53713FADAB25}" name="Catégorie"/>
     <tableColumn id="9" xr3:uid="{3327AB06-16A5-43C1-9A6C-CF851B135E2D}" name="Agriculture Bio"/>
-    <tableColumn id="8" xr3:uid="{49CA51DD-41A7-4500-B277-6CDA312A45FF}" name="Disponible à la vente_x000a_(si &quot;Non&quot;, les consommateurs ne peuvent pas commander le produit)"/>
     <tableColumn id="6" xr3:uid="{4151F915-395A-46D3-A6A1-23B1CAA9DC43}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -591,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE41FBF-0F39-4D6D-9EC2-F60889C1F878}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,12 +603,11 @@
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="45" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="45" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -641,14 +635,11 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="D2:D1048576" xr:uid="{158F52B8-4521-4DFE-85C4-7E1DDB94B372}">
@@ -663,7 +654,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="H2:H1048576" xr:uid="{363A8532-58B7-47B2-9B73-90212EFBEAE8}">
       <formula1>liste_categorie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:J1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cliquez sur la flèche à droite de la case" sqref="I2:I1048576" xr:uid="{4F5AC7B6-AFC9-4C28-A449-B46D8A9BCC11}">
       <formula1>liste_bool</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erreur" error="Attention, il faut saisir un nombre (entier ou décimal) supérieur à 0. Cliquez sur &quot;Rééssayer&quot; pour modifier votre saisie." sqref="F2:F1048576 C2:C1048576" xr:uid="{6C033349-5EF2-4B74-927B-A1C073480D73}">

</xml_diff>

<commit_message>
Update - Mise à jour du fichier import products
</commit_message>
<xml_diff>
--- a/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
+++ b/Sheaft.Resources/Excel/sheaft_catalogue_produits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\sheaft\api\Sheaft.Resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB5E5D7-853A-494A-9CA5-831B88C5893A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C78A8A-41E1-458D-9DFC-A53B3293D0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
+    <workbookView xWindow="4035" yWindow="3555" windowWidth="24660" windowHeight="12855" xr2:uid="{FC6F2FE0-A4D5-47D0-9EEA-C0DD31E43561}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Référence</t>
   </si>
@@ -125,6 +125,12 @@
   <si>
     <t>Nombre de pièces ou poids
 (si boîte, quantité contenue)</t>
+  </si>
+  <si>
+    <t>Mollusques et crustacés</t>
+  </si>
+  <si>
+    <t>Panier garni</t>
   </si>
 </sst>
 </file>
@@ -267,10 +273,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{482A5A29-7639-4322-B562-2426D46250A7}" name="Tableau5" displayName="Tableau5" ref="G1:G7" totalsRowShown="0">
-  <autoFilter ref="G1:G7" xr:uid="{C4CC0989-BC2B-4B26-8D92-EBAD3EF0C78D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G7">
-    <sortCondition ref="G2:G7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{482A5A29-7639-4322-B562-2426D46250A7}" name="Tableau5" displayName="Tableau5" ref="G1:G9" totalsRowShown="0">
+  <autoFilter ref="G1:G9" xr:uid="{C4CC0989-BC2B-4B26-8D92-EBAD3EF0C78D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G9">
+    <sortCondition ref="G1:G9"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{567C0C37-678B-423F-9212-65CEE0DFA9B1}" name="Catégorie"/>
@@ -589,7 +595,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,10 +677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372973B1-2516-4285-BAE1-16E251103327}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,11 +772,21 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>